<commit_message>
Added test cases for Profile and Ratings modules
Expanded Buggy Car Ratings coverage
</commit_message>
<xml_diff>
--- a/Buggy Car Rating.xlsx
+++ b/Buggy Car Rating.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L e n o v o\Documents\NSBM\3.1\SQA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L e n o v o\Documents\My Documents\Test Cases\Test-Cases_Buggy-Car-Rating\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{50C049C7-ED30-4B75-956C-284903BF9509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980AB482-E845-429D-93A4-A1E89CF2E438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{6450DB22-DEDA-42D4-BAF3-6A0AF00DAE9A}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="176">
   <si>
     <t>Project Name</t>
   </si>
@@ -454,6 +454,138 @@
   </si>
   <si>
     <t>Cars should reorder based on "Votes" in descending order.</t>
+  </si>
+  <si>
+    <t>Customer should be able enter their correct details</t>
+  </si>
+  <si>
+    <t>TC_PROFILE_001</t>
+  </si>
+  <si>
+    <t>Verify whether the basic details are already filled in with login details.</t>
+  </si>
+  <si>
+    <t>1. 1. Click “Profile"
+2. Check basic details</t>
+  </si>
+  <si>
+    <t>Checking whther the basic details are already filled in with login details.</t>
+  </si>
+  <si>
+    <t>The basic details are already filled in with login details.</t>
+  </si>
+  <si>
+    <t>Filled with details</t>
+  </si>
+  <si>
+    <t>TC_PROFILE_002</t>
+  </si>
+  <si>
+    <t>Verify whether gender can be selected.</t>
+  </si>
+  <si>
+    <t>Select gender "Female" or "Male".</t>
+  </si>
+  <si>
+    <t>1. Navigate to “Gender" field.
+2. Select gender</t>
+  </si>
+  <si>
+    <t>Select gender as user preference.</t>
+  </si>
+  <si>
+    <t>Selected.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify whether the customer can enter 18&lt;= age &lt;= 95 years. </t>
+  </si>
+  <si>
+    <t>The customer can enter 18&lt;= age &lt;= 95 years without any error messages.</t>
+  </si>
+  <si>
+    <t>1. Navigate to “Age" Field.
+2. Enter 18&lt;= values&lt;=95</t>
+  </si>
+  <si>
+    <t>Customer can enter values without any error messages.</t>
+  </si>
+  <si>
+    <t>No Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify whether the customer can't enter age &gt; 95 years. </t>
+  </si>
+  <si>
+    <t>The customer can't enter age&gt; 95 years without any error messages.</t>
+  </si>
+  <si>
+    <t>1. Navigate to “Age" Field.
+2. Enter values&gt;95</t>
+  </si>
+  <si>
+    <t>96, 100</t>
+  </si>
+  <si>
+    <t>Age must be in the range from 0 to 95</t>
+  </si>
+  <si>
+    <t>Display error message. "Age must be in the range from 18 to 95"</t>
+  </si>
+  <si>
+    <t>Age must be in the range from 18 to 95</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Error message has to be changed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify whether the customer can't enter age &lt;18 years. </t>
+  </si>
+  <si>
+    <t>The customer can't enter age&lt;18 years without any error messages.</t>
+  </si>
+  <si>
+    <t>18, 25, 50, 95</t>
+  </si>
+  <si>
+    <t>17, 0</t>
+  </si>
+  <si>
+    <t>No Error message displayed</t>
+  </si>
+  <si>
+    <t>Verify whether the phone number should be included with 10 characters.</t>
+  </si>
+  <si>
+    <t>The phone number should be included with 10 characters.</t>
+  </si>
+  <si>
+    <t>1. Navigate to “Age" Field.
+2. Enter values&lt;19</t>
+  </si>
+  <si>
+    <t>1. Navigate to “Phone number" Field.
+2. Enter Test datas.</t>
+  </si>
+  <si>
+    <t>0717334468, 098, 071234567890</t>
+  </si>
+  <si>
+    <t>If characters are higher or lower than 10, show error message</t>
+  </si>
+  <si>
+    <t>No Error message displayed in lower or higher than 10 characters</t>
+  </si>
+  <si>
+    <t>Show error.</t>
+  </si>
+  <si>
+    <t>Profile</t>
   </si>
 </sst>
 </file>
@@ -523,7 +655,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -547,6 +679,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1790,7 +1925,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2138,14 +2273,363 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCD70472-D8F0-44F0-B4C5-907E433A1EA1}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17:H17"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.21875" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" customWidth="1"/>
+    <col min="8" max="8" width="31" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="10" max="10" width="30.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="8">
+        <v>45829</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="8">
+        <v>45829</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="8">
+        <v>45829</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>